<commit_message>
added new figures for fiona's
</commit_message>
<xml_diff>
--- a/fiona/data.xlsx
+++ b/fiona/data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/j_igarashi/Documents/git/JinIgarashi/cacus-narok-figures/fiona/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0515B5-58F2-B847-956E-13508539A4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443D2BFC-93DB-E14C-B951-FBF160E9A9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{4C00E243-9F2A-B441-AADD-7B36CF36FAEE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{4C00E243-9F2A-B441-AADD-7B36CF36FAEE}"/>
   </bookViews>
   <sheets>
     <sheet name="cactus_data" sheetId="15" r:id="rId1"/>
     <sheet name="component_fsm" sheetId="16" r:id="rId2"/>
     <sheet name="component_fsm_empty_transport" sheetId="17" r:id="rId3"/>
+    <sheet name="fulllifecycle cost global" sheetId="18" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cactus_data!$A$1:$AR$126</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3198" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3264" uniqueCount="410">
   <si>
     <t>Infiltrating pit</t>
   </si>
@@ -1169,12 +1170,117 @@
   </si>
   <si>
     <t>Machine-powered aerobic waste water</t>
+  </si>
+  <si>
+    <t>Emptying and transport</t>
+  </si>
+  <si>
+    <t>Treatment (indicative)</t>
+  </si>
+  <si>
+    <t>Container aerobic FS treatment</t>
+  </si>
+  <si>
+    <t>Infiltrating pit aerobic FS treatment</t>
+  </si>
+  <si>
+    <t>Sealed tank with infiltration structure anaerobic FS treatment</t>
+  </si>
+  <si>
+    <t>Sealed tank without infiltration structure anaerobic FS treatment</t>
+  </si>
+  <si>
+    <t>Separate E&amp;T with transfer station</t>
+  </si>
+  <si>
+    <t>Manual emptying + machine powered transport</t>
+  </si>
+  <si>
+    <t>Human/machine powered E&amp;T with transfer station</t>
+  </si>
+  <si>
+    <t>Human powered E&amp;T</t>
+  </si>
+  <si>
+    <t>Machine powered E&amp;T</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Emptying type</t>
+  </si>
+  <si>
+    <t>Container aerobic FS treatment, Human/machine powered E&amp;T with transfer station</t>
+  </si>
+  <si>
+    <t>Container aerobic FS treatment, Manual emptying + machine powered transport</t>
+  </si>
+  <si>
+    <t>Container aerobic FS treatment, Separate E&amp;T with transfer station</t>
+  </si>
+  <si>
+    <t>Container aerobic FS treatment, Human powered E&amp;T</t>
+  </si>
+  <si>
+    <t>Container aerobic FS treatment, Machine powered E&amp;T</t>
+  </si>
+  <si>
+    <t>Infiltrating pit aerobic FS treatment, Separate E&amp;T with transfer station</t>
+  </si>
+  <si>
+    <t>Infiltrating pit aerobic FS treatment, Manual emptying + machine powered transport</t>
+  </si>
+  <si>
+    <t>Infiltrating pit aerobic FS treatment, Human/machine powered E&amp;T with transfer station</t>
+  </si>
+  <si>
+    <t>Sealed tank with infiltration structure anaerobic FS treatment, Separate E&amp;T with transfer station</t>
+  </si>
+  <si>
+    <t>Sealed tank without infiltration structure anaerobic FS treatment, Separate E&amp;T with transfer station</t>
+  </si>
+  <si>
+    <t>Sealed tank with infiltration structure anaerobic FS treatment, Manual emptying + machine powered transport</t>
+  </si>
+  <si>
+    <t>Sealed tank without infiltration structure anaerobic FS treatment, Manual emptying + machine powered transport</t>
+  </si>
+  <si>
+    <t>Sealed tank with infiltration structure anaerobic FS treatment, Human/machine powered E&amp;T with transfer station</t>
+  </si>
+  <si>
+    <t>Sealed tank without infiltration structure anaerobic FS treatment, Human/machine powered E&amp;T with transfer station</t>
+  </si>
+  <si>
+    <t>Infiltrating pit aerobic FS treatment, Human powered E&amp;T, Human powered E&amp;T</t>
+  </si>
+  <si>
+    <t>Sealed tank with infiltration structure anaerobic FS treatment, Human powered E&amp;T</t>
+  </si>
+  <si>
+    <t>Sealed tank without infiltration structure anaerobic FS treatment, Human powered E&amp;T</t>
+  </si>
+  <si>
+    <t>Infiltrating pit aerobic FS treatment, Machine powered E&amp;T, Machine powered E&amp;T</t>
+  </si>
+  <si>
+    <t>Sealed tank with infiltration structure anaerobic FS treatment, Machine powered E&amp;T</t>
+  </si>
+  <si>
+    <t>Sealed tank without infiltration structure anaerobic FS treatment, Machine powered E&amp;T</t>
+  </si>
+  <si>
+    <t>Container type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1204,12 +1310,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -27712,7 +27819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD6B218-87B5-E04A-92E3-FFAA50C27F19}">
   <dimension ref="A1:AR27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -31339,4 +31446,443 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91885CCD-4B56-AF43-8BEA-3FBB4AAD60BF}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="69.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>376</v>
+      </c>
+      <c r="F1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D2" s="3">
+        <v>127.49000000000001</v>
+      </c>
+      <c r="E2">
+        <v>34</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B3" t="s">
+        <v>378</v>
+      </c>
+      <c r="C3" t="s">
+        <v>383</v>
+      </c>
+      <c r="D3" s="3">
+        <v>127.49000000000001</v>
+      </c>
+      <c r="E3">
+        <v>56</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B4" t="s">
+        <v>378</v>
+      </c>
+      <c r="C4" t="s">
+        <v>384</v>
+      </c>
+      <c r="D4" s="3">
+        <v>127.49000000000001</v>
+      </c>
+      <c r="E4">
+        <v>101</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B5" t="s">
+        <v>378</v>
+      </c>
+      <c r="C5" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5" s="3">
+        <v>127.49000000000001</v>
+      </c>
+      <c r="E5">
+        <v>147</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>393</v>
+      </c>
+      <c r="B6" t="s">
+        <v>378</v>
+      </c>
+      <c r="C6" t="s">
+        <v>386</v>
+      </c>
+      <c r="D6" s="3">
+        <v>127.49000000000001</v>
+      </c>
+      <c r="E6">
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>394</v>
+      </c>
+      <c r="B7" t="s">
+        <v>379</v>
+      </c>
+      <c r="C7" t="s">
+        <v>382</v>
+      </c>
+      <c r="D7" s="3">
+        <v>412.34047619047618</v>
+      </c>
+      <c r="E7">
+        <v>34</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>395</v>
+      </c>
+      <c r="B8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C8" t="s">
+        <v>383</v>
+      </c>
+      <c r="D8" s="3">
+        <v>412.34047619047618</v>
+      </c>
+      <c r="E8">
+        <v>56</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>396</v>
+      </c>
+      <c r="B9" t="s">
+        <v>379</v>
+      </c>
+      <c r="C9" t="s">
+        <v>384</v>
+      </c>
+      <c r="D9" s="3">
+        <v>412.34047619047618</v>
+      </c>
+      <c r="E9">
+        <v>101</v>
+      </c>
+      <c r="F9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>403</v>
+      </c>
+      <c r="B10" t="s">
+        <v>379</v>
+      </c>
+      <c r="C10" t="s">
+        <v>385</v>
+      </c>
+      <c r="D10" s="3">
+        <v>412.34047619047618</v>
+      </c>
+      <c r="E10">
+        <v>147</v>
+      </c>
+      <c r="F10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>406</v>
+      </c>
+      <c r="B11" t="s">
+        <v>379</v>
+      </c>
+      <c r="C11" t="s">
+        <v>386</v>
+      </c>
+      <c r="D11" s="3">
+        <v>412.34047619047618</v>
+      </c>
+      <c r="E11">
+        <v>40</v>
+      </c>
+      <c r="F11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>397</v>
+      </c>
+      <c r="B12" t="s">
+        <v>380</v>
+      </c>
+      <c r="C12" t="s">
+        <v>382</v>
+      </c>
+      <c r="D12" s="3">
+        <v>472.51099999999997</v>
+      </c>
+      <c r="E12">
+        <v>34</v>
+      </c>
+      <c r="F12">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>399</v>
+      </c>
+      <c r="B13" t="s">
+        <v>380</v>
+      </c>
+      <c r="C13" t="s">
+        <v>383</v>
+      </c>
+      <c r="D13" s="3">
+        <v>472.51099999999997</v>
+      </c>
+      <c r="E13">
+        <v>56</v>
+      </c>
+      <c r="F13">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>401</v>
+      </c>
+      <c r="B14" t="s">
+        <v>380</v>
+      </c>
+      <c r="C14" t="s">
+        <v>384</v>
+      </c>
+      <c r="D14" s="3">
+        <v>472.51099999999997</v>
+      </c>
+      <c r="E14">
+        <v>101</v>
+      </c>
+      <c r="F14">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>404</v>
+      </c>
+      <c r="B15" t="s">
+        <v>380</v>
+      </c>
+      <c r="C15" t="s">
+        <v>385</v>
+      </c>
+      <c r="D15" s="3">
+        <v>472.51099999999997</v>
+      </c>
+      <c r="E15">
+        <v>147</v>
+      </c>
+      <c r="F15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>407</v>
+      </c>
+      <c r="B16" t="s">
+        <v>380</v>
+      </c>
+      <c r="C16" t="s">
+        <v>386</v>
+      </c>
+      <c r="D16" s="3">
+        <v>472.51099999999997</v>
+      </c>
+      <c r="E16">
+        <v>40</v>
+      </c>
+      <c r="F16">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>398</v>
+      </c>
+      <c r="B17" t="s">
+        <v>381</v>
+      </c>
+      <c r="C17" t="s">
+        <v>382</v>
+      </c>
+      <c r="D17" s="3">
+        <v>83.251111111111101</v>
+      </c>
+      <c r="E17">
+        <v>34</v>
+      </c>
+      <c r="F17">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>400</v>
+      </c>
+      <c r="B18" t="s">
+        <v>381</v>
+      </c>
+      <c r="C18" t="s">
+        <v>383</v>
+      </c>
+      <c r="D18" s="3">
+        <v>83.251111111111101</v>
+      </c>
+      <c r="E18">
+        <v>56</v>
+      </c>
+      <c r="F18">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>402</v>
+      </c>
+      <c r="B19" t="s">
+        <v>381</v>
+      </c>
+      <c r="C19" t="s">
+        <v>384</v>
+      </c>
+      <c r="D19" s="3">
+        <v>83.251111111111101</v>
+      </c>
+      <c r="E19">
+        <v>101</v>
+      </c>
+      <c r="F19">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>405</v>
+      </c>
+      <c r="B20" t="s">
+        <v>381</v>
+      </c>
+      <c r="C20" t="s">
+        <v>385</v>
+      </c>
+      <c r="D20" s="3">
+        <v>83.251111111111101</v>
+      </c>
+      <c r="E20">
+        <v>147</v>
+      </c>
+      <c r="F20">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>408</v>
+      </c>
+      <c r="B21" t="s">
+        <v>381</v>
+      </c>
+      <c r="C21" t="s">
+        <v>386</v>
+      </c>
+      <c r="D21" s="3">
+        <v>83.251111111111101</v>
+      </c>
+      <c r="E21">
+        <v>40</v>
+      </c>
+      <c r="F21">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>